<commit_message>
Corrected BOM for C1-C6
</commit_message>
<xml_diff>
--- a/documentation/reDIP-64-BOM.xlsx
+++ b/documentation/reDIP-64-BOM.xlsx
@@ -1660,14 +1660,14 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.10      $0.10
-    10   $0.03      $0.34
-    50   $0.02      $0.93
-   100   $0.02      $1.52
-   500   $0.01      $5.43
-  1000   $0.01      $8.54
-  2500   $0.01     $19.40
-  5000   $0.01     $35.70
- 15000   $0.01     $93.15</t>
+    10   $0.04      $0.38
+    50   $0.02      $1.03
+   100   $0.02      $1.68
+   500   $0.01      $6.00
+  1000   $0.01      $9.42
+  2500   $0.01     $21.42
+  5000   $0.01     $39.40
+ 15000   $0.01     $89.10</t>
         </r>
       </text>
     </comment>
@@ -1683,14 +1683,14 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-    10   £0.02      £0.20
-   100   £0.02      £1.59
-   150   £0.02      £2.39
-   500   £0.01      £3.80
-  2500   £0.01     £14.75
-  7500   £0.01     £43.50
- 15000   £0.00     £60.00
- 75000   £0.00    £292.50</t>
+    10   £0.05      £0.52
+   100   £0.03      £3.10
+   150   £0.03      £4.65
+   500   £0.03     £12.95
+  2500   £0.02     £51.00
+  7500   £0.02    £117.00
+ 15000   £0.00     £45.00
+ 75000   £0.00    £217.50</t>
         </r>
       </text>
     </comment>
@@ -1706,12 +1706,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-   100   $0.00      $0.33
-  1000   $0.00      $2.40
-  3000   $0.00      $6.90
- 10000   $0.00     $21.00
- 50000   $0.00    $100.00
-100000   $0.00    $200.00</t>
+   100   $0.00      $0.20
+  1000   $0.00      $1.40
+  3000   $0.00      $3.90
+ 10000   $0.00     $13.00
+ 50000   $0.00     $60.00
+100000   $0.00    $120.00</t>
         </r>
       </text>
     </comment>
@@ -1728,11 +1728,11 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.10      $0.10
-    10   $0.02      $0.18
-    50   $0.02      $0.90
-   100   $0.02      $1.50
-  1000   $0.01      $9.00
- 10000   $0.01     $70.00</t>
+    10   $0.02      $0.24
+    50   $0.02      $1.20
+   100   $0.01      $1.00
+  1000   $0.01      $6.00
+ 10000   $0.00     $40.00</t>
         </r>
       </text>
     </comment>
@@ -1748,11 +1748,14 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-    10   $0.03      $0.34
-    25   $0.03      $0.70
-    50   $0.02      $1.05
-   100   $0.02      $1.50
- 15000   $0.00     $75.00</t>
+    10   $0.04      $0.40
+    25   $0.03      $0.83
+    50   $0.02      $1.25
+   100   $0.02      $1.80
+   250   $0.02      $4.00
+   500   $0.01      $6.50
+  1000   $0.01     $10.00
+ 15000   $0.01     $90.00</t>
         </r>
       </text>
     </comment>
@@ -1768,8 +1771,29 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
- 15000   £0.00     £60.00
- 60000   £0.00    £240.00</t>
+   200   £0.00      £0.20
+  2000   £0.00      £6.00
+ 10000   £0.00     £30.00
+ 15000   £0.00     £45.00
+ 30000   £0.00     £90.00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (GBP):
+  Qty  -  Unit£  -  Ext£
+================
+   100   £0.01      £0.94
+  1000   £0.01      £6.25
+ 15000   £0.00     £39.60</t>
         </r>
       </text>
     </comment>
@@ -5526,7 +5550,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="427">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -5580,8 +5604,8 @@
   </si>
   <si>
     <t>C11,C15,C17,C22,C23,C25-C28,C30,C31,C44,C45,C48,C49,C52-C57,C59,C64,C65: 3.3V DC DERATED TO 0.1uF
-C60: 1.2V DC DERATED TO 0.1uF
-C61: 1.5V DC VAG DERATED TO 0.1uF</t>
+C61: 1.5V DC VAG DERATED TO 0.1uF
+C60: 1.2V DC DERATED TO 0.1uF</t>
   </si>
   <si>
     <t>C12,C13,C18,C19</t>
@@ -5647,8 +5671,8 @@
     <t>GRM033C80J105ME05D</t>
   </si>
   <si>
-    <t>C62,C63,C66,C67: 1.5V DC AUDIO
-C39: 1.2V DC</t>
+    <t>C39: 1.2V DC
+C62,C63,C66,C67: 1.5V DC AUDIO</t>
   </si>
   <si>
     <t>C1-C6</t>
@@ -5658,6 +5682,9 @@
   </si>
   <si>
     <t>CAP CER 100nF 6.3V 10% X5R 0201</t>
+  </si>
+  <si>
+    <t>GRM033R60J104KE19D</t>
   </si>
   <si>
     <t>C7-C10,C14,C16,C20,C21,C24,C29,C36-C38,C40-C43,C46,C47,C50,C51,C58</t>
@@ -6232,7 +6259,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>lø. 12. juni 2021 kl. 08.28 +0200</t>
+    <t>lø. 12. juni 2021 kl. 23.07 +0200</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -6247,7 +6274,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2021-06-12 08:28:45</t>
+    <t>2021-06-12 23:08:49</t>
   </si>
   <si>
     <t>Arrow</t>
@@ -6286,6 +6313,9 @@
     <t>490-13218-1-ND</t>
   </si>
   <si>
+    <t>490-3167-1-ND</t>
+  </si>
+  <si>
     <t>490-13230-1-ND</t>
   </si>
   <si>
@@ -6415,6 +6445,9 @@
     <t>3582762</t>
   </si>
   <si>
+    <t>1775994</t>
+  </si>
+  <si>
     <t>3238402</t>
   </si>
   <si>
@@ -6505,6 +6538,9 @@
     <t>C126630</t>
   </si>
   <si>
+    <t>C76928</t>
+  </si>
+  <si>
     <t>C335103</t>
   </si>
   <si>
@@ -6553,6 +6589,9 @@
     <t>81GRM033C80J105ME5D</t>
   </si>
   <si>
+    <t>81GRM033R60J104KE19</t>
+  </si>
+  <si>
     <t>81GRM035R60J475ME5D</t>
   </si>
   <si>
@@ -6667,6 +6706,9 @@
     <t>03AJ1531</t>
   </si>
   <si>
+    <t>51R6558</t>
+  </si>
+  <si>
     <t>34AH0743</t>
   </si>
   <si>
@@ -6752,6 +6794,9 @@
   </si>
   <si>
     <t>1851581</t>
+  </si>
+  <si>
+    <t>7235149</t>
   </si>
   <si>
     <t>1807476</t>
@@ -7430,13 +7475,13 @@
   <sheetData>
     <row r="1" spans="1:50">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J1" s="3">
         <v>100</v>
@@ -7444,13 +7489,13 @@
     </row>
     <row r="2" spans="1:50">
       <c r="A2" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J2" s="4">
         <f>TotalCost/BoardQty</f>
@@ -7459,13 +7504,13 @@
     </row>
     <row r="3" spans="1:50">
       <c r="A3" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J3" s="5">
         <f>SUM(J7:J51)</f>
@@ -7538,10 +7583,10 @@
     </row>
     <row r="4" spans="1:50">
       <c r="A4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:50">
@@ -7558,56 +7603,56 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
       <c r="U5" s="10" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="11" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="12" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AF5" s="12"/>
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="13" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="AK5" s="13"/>
       <c r="AL5" s="13"/>
       <c r="AM5" s="13"/>
       <c r="AN5" s="13"/>
       <c r="AO5" s="14" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="AP5" s="14"/>
       <c r="AQ5" s="14"/>
       <c r="AR5" s="14"/>
       <c r="AS5" s="14"/>
       <c r="AT5" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="AU5" s="15"/>
       <c r="AV5" s="15"/>
@@ -7646,10 +7691,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M6" s="16" t="s">
         <v>8</v>
@@ -7658,13 +7703,13 @@
         <v>9</v>
       </c>
       <c r="O6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>8</v>
@@ -7673,13 +7718,13 @@
         <v>9</v>
       </c>
       <c r="T6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="V6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="W6" s="16" t="s">
         <v>8</v>
@@ -7688,13 +7733,13 @@
         <v>9</v>
       </c>
       <c r="Y6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="Z6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="AA6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="AB6" s="16" t="s">
         <v>8</v>
@@ -7703,13 +7748,13 @@
         <v>9</v>
       </c>
       <c r="AD6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AF6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="AE6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="AF6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>8</v>
@@ -7718,13 +7763,13 @@
         <v>9</v>
       </c>
       <c r="AI6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AJ6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AK6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="AJ6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="AK6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="AL6" s="16" t="s">
         <v>8</v>
@@ -7733,13 +7778,13 @@
         <v>9</v>
       </c>
       <c r="AN6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AO6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AP6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="AO6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="AP6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="AQ6" s="16" t="s">
         <v>8</v>
@@ -7748,13 +7793,13 @@
         <v>9</v>
       </c>
       <c r="AS6" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AT6" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="AU6" s="16" t="s">
         <v>242</v>
-      </c>
-      <c r="AT6" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="AU6" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="AV6" s="16" t="s">
         <v>8</v>
@@ -7763,7 +7808,7 @@
         <v>9</v>
       </c>
       <c r="AX6" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:50">
@@ -7812,7 +7857,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="19" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="U7" s="17">
         <v>120000</v>
@@ -7826,7 +7871,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="Z7" s="17">
         <v>25800</v>
@@ -7840,7 +7885,7 @@
         <v>0</v>
       </c>
       <c r="AD7" s="19" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="AE7" s="17">
         <v>920775</v>
@@ -7854,7 +7899,7 @@
         <v>0</v>
       </c>
       <c r="AI7" s="19" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AJ7" s="17">
         <v>120000</v>
@@ -7868,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="AN7" s="19" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="AO7" s="17">
         <v>7000</v>
@@ -7882,7 +7927,7 @@
         <v>0</v>
       </c>
       <c r="AS7" s="19" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:50">
@@ -7920,7 +7965,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R8" s="18">
         <f>iferror(lookup(if(Q8="",H8,Q8),{0,1,10,50,100,500,1000,2500,5000,10000},{0.0,0.29,0.198,0.119,0.1005,0.06876,0.06084,0.05819,0.0529,0.05026}),"")</f>
@@ -7931,7 +7976,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="U8" s="17">
         <v>4340</v>
@@ -7945,7 +7990,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="19" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="Z8" s="17">
         <v>9720</v>
@@ -7959,10 +8004,10 @@
         <v>0</v>
       </c>
       <c r="AD8" s="19" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="AE8" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG8" s="18">
         <f>iferror(lookup(if(AF8="",H8,AF8),{0,1,10,50,100,1000,10000},{0.0,0.26,0.174,0.174,0.099,0.061,0.043}),"")</f>
@@ -7973,7 +8018,7 @@
         <v>0</v>
       </c>
       <c r="AI8" s="19" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AJ8" s="17">
         <v>4340</v>
@@ -7987,7 +8032,7 @@
         <v>0</v>
       </c>
       <c r="AN8" s="19" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:50">
@@ -8036,10 +8081,10 @@
         <v>0</v>
       </c>
       <c r="T9" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="U9" s="20" t="s">
         <v>248</v>
-      </c>
-      <c r="U9" s="20" t="s">
-        <v>247</v>
       </c>
       <c r="W9" s="18">
         <f>iferror(USD_GBP*lookup(if(V9="",H9,V9),{0,1,10,100,150,500,1000,2000,4000,20000},{0.0,0.287,0.287,0.179,0.179,0.135,0.116,0.0956,0.0797,0.0683}),"")</f>
@@ -8050,7 +8095,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="19" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AE9" s="17">
         <v>901015</v>
@@ -8064,10 +8109,10 @@
         <v>0</v>
       </c>
       <c r="AI9" s="19" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="AJ9" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL9" s="18">
         <f>iferror(lookup(if(AK9="",H9,AK9),{0,1,10,25,50,100,4000,8000},{0.0,0.42,0.42,0.372,0.324,0.276,0.117,0.113}),"")</f>
@@ -8078,7 +8123,7 @@
         <v>0</v>
       </c>
       <c r="AN9" s="19" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:50">
@@ -8127,10 +8172,10 @@
         <v>0</v>
       </c>
       <c r="T10" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="U10" s="20" t="s">
         <v>248</v>
-      </c>
-      <c r="U10" s="20" t="s">
-        <v>247</v>
       </c>
       <c r="W10" s="18">
         <f>iferror(USD_GBP*lookup(if(V10="",H10,V10),{0,1,10,100,150,500,1000,2000,4000,20000},{0.0,0.287,0.287,0.179,0.179,0.135,0.116,0.0956,0.0797,0.0683}),"")</f>
@@ -8141,7 +8186,7 @@
         <v>0</v>
       </c>
       <c r="Y10" s="19" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AE10" s="17">
         <v>901015</v>
@@ -8155,10 +8200,10 @@
         <v>0</v>
       </c>
       <c r="AI10" s="19" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="AJ10" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL10" s="18">
         <f>iferror(lookup(if(AK10="",H10,AK10),{0,1,10,25,50,100,4000,8000},{0.0,0.42,0.42,0.372,0.324,0.276,0.117,0.113}),"")</f>
@@ -8169,7 +8214,7 @@
         <v>0</v>
       </c>
       <c r="AN10" s="19" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:50">
@@ -8207,7 +8252,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R11" s="18">
         <f>iferror(lookup(if(Q11="",H11,Q11),{0,1,10,50,100,500,1000,4000},{0.0,0.48,0.339,0.2566,0.2235,0.16552,0.1407,0.12415}),"")</f>
@@ -8218,10 +8263,10 @@
         <v>0</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="U11" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W11" s="18">
         <f>iferror(USD_GBP*lookup(if(V11="",H11,V11),{0,1,10,100,150,500,1000,2000,4000,20000},{0.0,0.288,0.288,0.18,0.18,0.136,0.116,0.096,0.08,0.0686}),"")</f>
@@ -8232,7 +8277,7 @@
         <v>0</v>
       </c>
       <c r="Y11" s="19" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="Z11" s="17">
         <v>7140</v>
@@ -8246,10 +8291,10 @@
         <v>0</v>
       </c>
       <c r="AD11" s="19" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="AE11" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG11" s="18">
         <f>iferror(lookup(if(AF11="",H11,AF11),{0,1,10,50,100,1000,10000},{0.0,0.54,0.39,0.39,0.257,0.162,0.126}),"")</f>
@@ -8260,10 +8305,10 @@
         <v>0</v>
       </c>
       <c r="AI11" s="19" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="AJ11" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL11" s="18">
         <f>iferror(lookup(if(AK11="",H11,AK11),{0,1,10,25,50,100,250},{0.0,0.39,0.39,0.346,0.301,0.257,0.228}),"")</f>
@@ -8274,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="AN11" s="19" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:50">
@@ -8312,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R12" s="18">
         <f>iferror(lookup(if(Q12="",H12,Q12),{0,1,10,50,100,500,1000,2500,5000,15000},{0.0,0.25,0.172,0.115,0.0978,0.069,0.06038,0.0575,0.05319,0.04773}),"")</f>
@@ -8323,10 +8368,10 @@
         <v>0</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="U12" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W12" s="18">
         <f>iferror(USD_GBP*lookup(if(V12="",H12,V12),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.218,0.218,0.137,0.137,0.103,0.0727,0.0606,0.0594,0.051}),"")</f>
@@ -8337,10 +8382,10 @@
         <v>0</v>
       </c>
       <c r="Y12" s="19" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AE12" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG12" s="18">
         <f>iferror(lookup(if(AF12="",H12,AF12),{0,1,10,50,100,1000,10000},{0.0,0.24,0.11,0.11,0.094,0.058,0.051}),"")</f>
@@ -8351,10 +8396,10 @@
         <v>0</v>
       </c>
       <c r="AI12" s="19" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="AJ12" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL12" s="18">
         <f>iferror(lookup(if(AK12="",H12,AK12),{0,1,10,25,50,100,15000},{0.0,0.121,0.121,0.113,0.105,0.097,0.053}),"")</f>
@@ -8365,7 +8410,7 @@
         <v>0</v>
       </c>
       <c r="AN12" s="19" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:50">
@@ -8385,7 +8430,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="H13" s="17">
         <f>BoardQty*6</f>
@@ -8400,10 +8445,10 @@
         <v>0</v>
       </c>
       <c r="P13" s="17">
-        <v>2579801</v>
+        <v>1851413</v>
       </c>
       <c r="R13" s="18">
-        <f>iferror(lookup(if(Q13="",H13,Q13),{0,1,10,50,100,500,1000,2500,5000,15000},{0.0,0.1,0.034,0.0186,0.0152,0.01086,0.00854,0.00776,0.00714,0.00621}),"")</f>
+        <f>iferror(lookup(if(Q13="",H13,Q13),{0,1,10,50,100,500,1000,2500,5000,15000},{0.0,0.1,0.038,0.0206,0.0168,0.012,0.00942,0.00857,0.00788,0.00594}),"")</f>
         <v>0</v>
       </c>
       <c r="S13" s="18">
@@ -8411,13 +8456,13 @@
         <v>0</v>
       </c>
       <c r="T13" s="19" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="U13" s="17">
-        <v>120000</v>
+        <v>105000</v>
       </c>
       <c r="W13" s="18">
-        <f>iferror(USD_GBP*lookup(if(V13="",H13,V13),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.0202,0.0202,0.0159,0.0159,0.0076,0.0059,0.0058,0.004,0.0039}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(V13="",H13,V13),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.0517,0.0517,0.031,0.031,0.0259,0.0204,0.0156,0.003,0.0029}),"")</f>
         <v>0</v>
       </c>
       <c r="X13" s="18">
@@ -8425,13 +8470,13 @@
         <v>0</v>
       </c>
       <c r="Y13" s="19" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="Z13" s="17">
-        <v>25800</v>
+        <v>2246700</v>
       </c>
       <c r="AB13" s="18">
-        <f>iferror(lookup(if(AA13="",H13,AA13),{0,1,100,1000,3000,10000,50000,100000},{0.0,0.0033,0.0033,0.0024,0.0023,0.0021,0.002,0.002}),"")</f>
+        <f>iferror(lookup(if(AA13="",H13,AA13),{0,1,100,1000,3000,10000,50000,100000},{0.0,0.002,0.002,0.0014,0.0013,0.0013,0.0012,0.0012}),"")</f>
         <v>0</v>
       </c>
       <c r="AC13" s="18">
@@ -8439,13 +8484,13 @@
         <v>0</v>
       </c>
       <c r="AD13" s="19" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="AE13" s="17">
-        <v>920775</v>
+        <v>1793383</v>
       </c>
       <c r="AG13" s="18">
-        <f>iferror(lookup(if(AF13="",H13,AF13),{0,1,10,50,100,1000,10000},{0.0,0.1,0.018,0.018,0.015,0.009,0.007}),"")</f>
+        <f>iferror(lookup(if(AF13="",H13,AF13),{0,1,10,50,100,1000,10000},{0.0,0.1,0.024,0.024,0.01,0.006,0.004}),"")</f>
         <v>0</v>
       </c>
       <c r="AH13" s="18">
@@ -8453,13 +8498,13 @@
         <v>0</v>
       </c>
       <c r="AI13" s="19" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="AJ13" s="17">
-        <v>120000</v>
+        <v>105000</v>
       </c>
       <c r="AL13" s="18">
-        <f>iferror(lookup(if(AK13="",H13,AK13),{0,1,10,25,50,100,15000},{0.0,0.034,0.034,0.028,0.021,0.015,0.005}),"")</f>
+        <f>iferror(lookup(if(AK13="",H13,AK13),{0,1,10,25,50,100,250,500,1000,15000},{0.0,0.04,0.04,0.033,0.025,0.018,0.016,0.013,0.01,0.006}),"")</f>
         <v>0</v>
       </c>
       <c r="AM13" s="18">
@@ -8467,13 +8512,13 @@
         <v>0</v>
       </c>
       <c r="AN13" s="19" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="AO13" s="17">
-        <v>7000</v>
+        <v>12800</v>
       </c>
       <c r="AQ13" s="18">
-        <f>iferror(USD_GBP*lookup(if(AP13="",H13,AP13),{0,1,15000,60000},{0.0,0.004,0.004,0.004}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(AP13="",H13,AP13),{0,1,200,2000,10000,15000,30000},{0.0,0.001,0.001,0.003,0.003,0.003,0.003}),"")</f>
         <v>0</v>
       </c>
       <c r="AR13" s="18">
@@ -8481,21 +8526,35 @@
         <v>0</v>
       </c>
       <c r="AS13" s="19" t="s">
-        <v>406</v>
+        <v>413</v>
+      </c>
+      <c r="AT13" s="17">
+        <v>23900</v>
+      </c>
+      <c r="AV13" s="18">
+        <f>iferror(USD_GBP*lookup(if(AU13="",H13,AU13),{0,1,100,1000,15000},{0.0,0.00944,0.00944,0.00625,0.00264}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AW13" s="18">
+        <f>iferror(if(AU13="",H13,AU13)*AV13,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AX13" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:50">
       <c r="A14" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>14</v>
@@ -8504,7 +8563,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H14" s="17">
         <f>BoardQty*22</f>
@@ -8519,7 +8578,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R14" s="18">
         <f>iferror(lookup(if(Q14="",H14,Q14),{0,1,10,50,100,500,1000,2500,5000,10000},{0.0,0.44,0.307,0.215,0.1842,0.13818,0.11668,0.11054,0.1044,0.09826}),"")</f>
@@ -8530,10 +8589,10 @@
         <v>0</v>
       </c>
       <c r="T14" s="19" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="U14" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W14" s="18">
         <f>iferror(USD_GBP*lookup(if(V14="",H14,V14),{0,1,10,100,150,500,2500,5000,10000,50000},{0.0,0.187,0.187,0.151,0.151,0.0842,0.0797,0.074,0.0718,0.0615}),"")</f>
@@ -8544,7 +8603,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="19" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="Z14" s="17">
         <v>267315</v>
@@ -8558,10 +8617,10 @@
         <v>0</v>
       </c>
       <c r="AD14" s="19" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="AE14" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG14" s="18">
         <f>iferror(lookup(if(AF14="",H14,AF14),{0,1,10,50,100,1000,10000},{0.0,0.42,0.206,0.206,0.177,0.112,0.094}),"")</f>
@@ -8572,10 +8631,10 @@
         <v>0</v>
       </c>
       <c r="AI14" s="19" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="AJ14" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL14" s="18">
         <f>iferror(lookup(if(AK14="",H14,AK14),{0,1,10,25,50,100,10000},{0.0,0.227,0.227,0.216,0.205,0.194,0.11}),"")</f>
@@ -8586,27 +8645,27 @@
         <v>0</v>
       </c>
       <c r="AN14" s="19" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:50">
       <c r="A15" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" s="17">
         <f>BoardQty*1</f>
@@ -8632,7 +8691,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="U15" s="17">
         <v>7740</v>
@@ -8646,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="Y15" s="19" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="AE15" s="17">
         <v>6160</v>
@@ -8660,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="AI15" s="19" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="AJ15" s="17">
         <v>7740</v>
@@ -8674,27 +8733,27 @@
         <v>0</v>
       </c>
       <c r="AN15" s="19" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:50">
       <c r="A16" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H16" s="17">
         <f>BoardQty*1</f>
@@ -8720,7 +8779,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="19" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AE16" s="17">
         <v>2192</v>
@@ -8734,7 +8793,7 @@
         <v>0</v>
       </c>
       <c r="AI16" s="19" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="AJ16" s="17">
         <v>9000</v>
@@ -8748,7 +8807,7 @@
         <v>0</v>
       </c>
       <c r="AN16" s="19" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="AO16" s="17">
         <v>10820</v>
@@ -8762,27 +8821,27 @@
         <v>0</v>
       </c>
       <c r="AS16" s="19" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:50">
       <c r="A17" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H17" s="17">
         <f>BoardQty*1</f>
@@ -8808,7 +8867,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="19" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AE17" s="17">
         <v>12139</v>
@@ -8822,7 +8881,7 @@
         <v>0</v>
       </c>
       <c r="AI17" s="19" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="AO17" s="17">
         <v>4800</v>
@@ -8836,27 +8895,27 @@
         <v>0</v>
       </c>
       <c r="AS17" s="19" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
     </row>
     <row r="18" spans="1:50">
       <c r="A18" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H18" s="17">
         <f>BoardQty*1</f>
@@ -8871,7 +8930,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R18" s="18">
         <f>iferror(lookup(if(Q18="",H18,Q18),{0,1,10,100,500,1000,2000,8000,16000,24000,56000},{0.0,0.51,0.382,0.2163,0.14322,0.1098,0.09548,0.08593,0.07638,0.07161,0.0651}),"")</f>
@@ -8882,10 +8941,10 @@
         <v>0</v>
       </c>
       <c r="T18" s="19" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="U18" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W18" s="18">
         <f>iferror(USD_GBP*lookup(if(V18="",H18,V18),{0,1,5,10,100,500,1000},{0.0,0.481,0.481,0.311,0.155,0.119,0.0725}),"")</f>
@@ -8896,10 +8955,10 @@
         <v>0</v>
       </c>
       <c r="Y18" s="19" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="AE18" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG18" s="18">
         <f>iferror(lookup(if(AF18="",H18,AF18),{0,1,10,50,100,1000,10000},{0.0,0.44,0.314,0.314,0.178,0.095,0.071}),"")</f>
@@ -8910,10 +8969,10 @@
         <v>0</v>
       </c>
       <c r="AI18" s="19" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="AJ18" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL18" s="18">
         <f>iferror(lookup(if(AK18="",H18,AK18),{0,1,5,10,100,500,1000,2500},{0.0,0.544,0.544,0.38,0.182,0.162,0.142,0.124}),"")</f>
@@ -8924,30 +8983,30 @@
         <v>0</v>
       </c>
       <c r="AN18" s="19" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:50">
       <c r="A19" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="F19" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>74</v>
-      </c>
       <c r="G19" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H19" s="17">
         <f>BoardQty*1</f>
@@ -8973,10 +9032,10 @@
         <v>0</v>
       </c>
       <c r="T19" s="19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="U19" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W19" s="18">
         <f>iferror(USD_GBP*lookup(if(V19="",H19,V19),{0,1,10,100,500},{0.0,0.683,0.451,0.347,0.299}),"")</f>
@@ -8987,10 +9046,10 @@
         <v>0</v>
       </c>
       <c r="Y19" s="19" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="AE19" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG19" s="18">
         <f>iferror(lookup(if(AF19="",H19,AF19),{0,1,10,50,100,1000,10000},{0.0,0.68,0.441,0.441,0.289,0.228,0.186}),"")</f>
@@ -9001,10 +9060,10 @@
         <v>0</v>
       </c>
       <c r="AI19" s="19" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="AJ19" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL19" s="18">
         <f>iferror(lookup(if(AK19="",H19,AK19),{0,1,10000},{0.0,0.222,0.222}),"")</f>
@@ -9015,10 +9074,10 @@
         <v>0</v>
       </c>
       <c r="AN19" s="19" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="AT19" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AV19" s="18">
         <f>iferror(USD_GBP*lookup(if(AU19="",H19,AU19),{0,1,5,25,100,500},{0.0,0.5821,0.2619,0.2037,0.1732,0.1579}),"")</f>
@@ -9029,27 +9088,27 @@
         <v>0</v>
       </c>
       <c r="AX19" s="19" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:50">
       <c r="A20" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H20" s="17">
         <f>BoardQty*4</f>
@@ -9064,7 +9123,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R20" s="18">
         <f>iferror(lookup(if(Q20="",H20,Q20),{0,1,10,25,50,100,250,500,1000,4000,8000,12000,28000},{0.0,0.1,0.079,0.072,0.0648,0.0475,0.03456,0.03168,0.02736,0.02304,0.02088,0.02016,0.01915}),"")</f>
@@ -9075,7 +9134,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="19" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="U20" s="17">
         <v>4729</v>
@@ -9089,7 +9148,7 @@
         <v>0</v>
       </c>
       <c r="Y20" s="19" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="Z20" s="17">
         <v>56350</v>
@@ -9103,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="AD20" s="19" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AE20" s="17">
         <v>6945</v>
@@ -9117,10 +9176,10 @@
         <v>0</v>
       </c>
       <c r="AI20" s="19" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="AJ20" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL20" s="18">
         <f>iferror(lookup(if(AK20="",H20,AK20),{0,1,10,25,50,100},{0.0,0.1,0.052,0.046,0.041,0.035}),"")</f>
@@ -9131,7 +9190,7 @@
         <v>0</v>
       </c>
       <c r="AN20" s="19" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="AO20" s="17">
         <v>6500</v>
@@ -9145,7 +9204,7 @@
         <v>0</v>
       </c>
       <c r="AS20" s="19" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="AT20" s="17">
         <v>1000</v>
@@ -9159,27 +9218,27 @@
         <v>0</v>
       </c>
       <c r="AX20" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:50">
       <c r="A21" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H21" s="17">
         <f>BoardQty*1</f>
@@ -9205,7 +9264,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="19" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="AE21" s="17">
         <v>453</v>
@@ -9219,27 +9278,27 @@
         <v>0</v>
       </c>
       <c r="AI21" s="19" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:50">
       <c r="A22" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H22" s="17">
         <f>BoardQty*2</f>
@@ -9265,27 +9324,27 @@
         <v>0</v>
       </c>
       <c r="T22" s="19" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:50">
       <c r="A23" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H23" s="17">
         <f>BoardQty*1</f>
@@ -9311,27 +9370,27 @@
         <v>0</v>
       </c>
       <c r="T23" s="19" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:50">
       <c r="A24" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H24" s="17">
         <f>BoardQty*3</f>
@@ -9357,27 +9416,27 @@
         <v>0</v>
       </c>
       <c r="T24" s="19" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:50">
       <c r="A25" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H25" s="17">
         <f>BoardQty*1</f>
@@ -9392,7 +9451,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R25" s="18">
         <f>iferror(lookup(if(Q25="",H25,Q25),{0,1,10000},{0.0,0.03532,0.03532}),"")</f>
@@ -9403,7 +9462,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="19" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AE25" s="17">
         <v>10000</v>
@@ -9417,27 +9476,27 @@
         <v>0</v>
       </c>
       <c r="AI25" s="19" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:50">
       <c r="A26" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H26" s="17">
         <f>BoardQty*1</f>
@@ -9463,10 +9522,10 @@
         <v>0</v>
       </c>
       <c r="T26" s="19" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="U26" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W26" s="18">
         <f>iferror(USD_GBP*lookup(if(V26="",H26,V26),{0,1,30000},{0.0,0.0064,0.0064}),"")</f>
@@ -9477,7 +9536,7 @@
         <v>0</v>
       </c>
       <c r="Y26" s="19" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="AE26" s="17">
         <v>80005</v>
@@ -9491,13 +9550,13 @@
         <v>0</v>
       </c>
       <c r="AI26" s="19" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="AJ26" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN26" s="19" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="AO26" s="17">
         <v>28000</v>
@@ -9511,27 +9570,27 @@
         <v>0</v>
       </c>
       <c r="AS26" s="19" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
     </row>
     <row r="27" spans="1:50">
       <c r="A27" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H27" s="17">
         <f>BoardQty*2</f>
@@ -9557,10 +9616,10 @@
         <v>0</v>
       </c>
       <c r="T27" s="19" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="U27" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W27" s="18">
         <f>iferror(USD_GBP*lookup(if(V27="",H27,V27),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -9571,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="Y27" s="19" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AE27" s="17">
         <v>24546</v>
@@ -9585,10 +9644,10 @@
         <v>0</v>
       </c>
       <c r="AI27" s="19" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="AJ27" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL27" s="18">
         <f>iferror(lookup(if(AK27="",H27,AK27),{0,1,15000,30000},{0.0,0.005,0.005,0.004}),"")</f>
@@ -9599,7 +9658,7 @@
         <v>0</v>
       </c>
       <c r="AN27" s="19" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="AO27" s="17">
         <v>38000</v>
@@ -9613,27 +9672,27 @@
         <v>0</v>
       </c>
       <c r="AS27" s="19" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:50">
       <c r="A28" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H28" s="17">
         <f>BoardQty*1</f>
@@ -9659,10 +9718,10 @@
         <v>0</v>
       </c>
       <c r="T28" s="19" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="U28" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W28" s="18">
         <f>iferror(USD_GBP*lookup(if(V28="",H28,V28),{0,1,30000},{0.0,0.0056,0.0056}),"")</f>
@@ -9673,7 +9732,7 @@
         <v>0</v>
       </c>
       <c r="Y28" s="19" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="AE28" s="17">
         <v>63697</v>
@@ -9687,27 +9746,27 @@
         <v>0</v>
       </c>
       <c r="AI28" s="19" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="1:50">
       <c r="A29" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H29" s="17">
         <f>BoardQty*5</f>
@@ -9733,10 +9792,10 @@
         <v>0</v>
       </c>
       <c r="T29" s="19" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="U29" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W29" s="18">
         <f>iferror(USD_GBP*lookup(if(V29="",H29,V29),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.04,0.04,0.024,0.024,0.018,0.012,0.009,0.007,0.0046}),"")</f>
@@ -9747,10 +9806,10 @@
         <v>0</v>
       </c>
       <c r="Y29" s="19" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="AE29" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG29" s="18">
         <f>iferror(lookup(if(AF29="",H29,AF29),{0,1,10,50,100,1000,10000},{0.0,0.1,0.028,0.028,0.012,0.006,0.004}),"")</f>
@@ -9761,7 +9820,7 @@
         <v>0</v>
       </c>
       <c r="AI29" s="19" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="AJ29" s="17">
         <v>60000</v>
@@ -9775,7 +9834,7 @@
         <v>0</v>
       </c>
       <c r="AN29" s="19" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="AO29" s="17">
         <v>24000</v>
@@ -9789,27 +9848,27 @@
         <v>0</v>
       </c>
       <c r="AS29" s="19" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="1:50">
       <c r="A30" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H30" s="17">
         <f>BoardQty*1</f>
@@ -9835,10 +9894,10 @@
         <v>0</v>
       </c>
       <c r="T30" s="19" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="U30" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W30" s="18">
         <f>iferror(USD_GBP*lookup(if(V30="",H30,V30),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -9849,7 +9908,7 @@
         <v>0</v>
       </c>
       <c r="Y30" s="19" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="Z30" s="17">
         <v>14450</v>
@@ -9863,7 +9922,7 @@
         <v>0</v>
       </c>
       <c r="AD30" s="19" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="AE30" s="17">
         <v>7006</v>
@@ -9877,33 +9936,33 @@
         <v>0</v>
       </c>
       <c r="AI30" s="19" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="AJ30" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AN30" s="19" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:50">
       <c r="A31" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H31" s="17">
         <f>BoardQty*3</f>
@@ -9929,10 +9988,10 @@
         <v>0</v>
       </c>
       <c r="T31" s="19" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="U31" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W31" s="18">
         <f>iferror(USD_GBP*lookup(if(V31="",H31,V31),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -9943,7 +10002,7 @@
         <v>0</v>
       </c>
       <c r="Y31" s="19" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="AE31" s="17">
         <v>3126</v>
@@ -9957,10 +10016,10 @@
         <v>0</v>
       </c>
       <c r="AI31" s="19" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="AJ31" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL31" s="18">
         <f>iferror(lookup(if(AK31="",H31,AK31),{0,1,15000},{0.0,0.006,0.006}),"")</f>
@@ -9971,27 +10030,27 @@
         <v>0</v>
       </c>
       <c r="AN31" s="19" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:50">
       <c r="A32" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H32" s="17">
         <f>BoardQty*2</f>
@@ -10017,10 +10076,10 @@
         <v>0</v>
       </c>
       <c r="T32" s="19" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="U32" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W32" s="18">
         <f>iferror(USD_GBP*lookup(if(V32="",H32,V32),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -10031,7 +10090,7 @@
         <v>0</v>
       </c>
       <c r="Y32" s="19" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="Z32" s="17">
         <v>14500</v>
@@ -10045,7 +10104,7 @@
         <v>0</v>
       </c>
       <c r="AD32" s="19" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="AE32" s="17">
         <v>22648</v>
@@ -10059,10 +10118,10 @@
         <v>0</v>
       </c>
       <c r="AI32" s="19" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="AJ32" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL32" s="18">
         <f>iferror(lookup(if(AK32="",H32,AK32),{0,1,135000},{0.0,0.004,0.004}),"")</f>
@@ -10073,7 +10132,7 @@
         <v>0</v>
       </c>
       <c r="AN32" s="19" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="AO32" s="17">
         <v>19000</v>
@@ -10087,27 +10146,27 @@
         <v>0</v>
       </c>
       <c r="AS32" s="19" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:50">
       <c r="A33" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H33" s="17">
         <f>BoardQty*3</f>
@@ -10122,7 +10181,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R33" s="18">
         <f>iferror(lookup(if(Q33="",H33,Q33),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.053,0.0217,0.00975,0.00846,0.00699,0.00607}),"")</f>
@@ -10133,7 +10192,7 @@
         <v>0</v>
       </c>
       <c r="T33" s="19" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="U33" s="17">
         <v>1646</v>
@@ -10147,7 +10206,7 @@
         <v>0</v>
       </c>
       <c r="Y33" s="19" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="Z33" s="17">
         <v>50</v>
@@ -10161,7 +10220,7 @@
         <v>0</v>
       </c>
       <c r="AD33" s="19" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="AE33" s="17">
         <v>5370</v>
@@ -10175,7 +10234,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="19" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="AJ33" s="17">
         <v>881</v>
@@ -10189,7 +10248,7 @@
         <v>0</v>
       </c>
       <c r="AN33" s="19" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="AO33" s="17">
         <v>26000</v>
@@ -10203,27 +10262,27 @@
         <v>0</v>
       </c>
       <c r="AS33" s="19" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:50">
       <c r="A34" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H34" s="17">
         <f>BoardQty*4</f>
@@ -10238,7 +10297,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R34" s="18">
         <f>iferror(lookup(if(Q34="",H34,Q34),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.028,0.0115,0.00518,0.0045,0.00371,0.00323}),"")</f>
@@ -10249,10 +10308,10 @@
         <v>0</v>
       </c>
       <c r="T34" s="19" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="U34" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W34" s="18">
         <f>iferror(USD_GBP*lookup(if(V34="",H34,V34),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -10263,7 +10322,7 @@
         <v>0</v>
       </c>
       <c r="Y34" s="19" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="Z34" s="17">
         <v>3200</v>
@@ -10277,7 +10336,7 @@
         <v>0</v>
       </c>
       <c r="AD34" s="19" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="AE34" s="17">
         <v>47058</v>
@@ -10291,10 +10350,10 @@
         <v>0</v>
       </c>
       <c r="AI34" s="19" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="AJ34" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL34" s="18">
         <f>iferror(lookup(if(AK34="",H34,AK34),{0,1,45000},{0.0,0.004,0.004}),"")</f>
@@ -10305,27 +10364,27 @@
         <v>0</v>
       </c>
       <c r="AN34" s="19" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:50">
       <c r="A35" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C35" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="H35" s="17">
         <f>BoardQty*1</f>
@@ -10351,7 +10410,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="19" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="U35" s="17">
         <v>679</v>
@@ -10365,7 +10424,7 @@
         <v>0</v>
       </c>
       <c r="Y35" s="19" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="Z35" s="17">
         <v>18022</v>
@@ -10379,7 +10438,7 @@
         <v>0</v>
       </c>
       <c r="AD35" s="19" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="AE35" s="17">
         <v>11251</v>
@@ -10393,7 +10452,7 @@
         <v>0</v>
       </c>
       <c r="AI35" s="19" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="AJ35" s="17">
         <v>7019</v>
@@ -10407,7 +10466,7 @@
         <v>0</v>
       </c>
       <c r="AN35" s="19" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="AT35" s="17">
         <v>2875</v>
@@ -10421,27 +10480,27 @@
         <v>0</v>
       </c>
       <c r="AX35" s="19" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="1:50">
       <c r="A36" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H36" s="17">
         <f>BoardQty*1</f>
@@ -10456,7 +10515,7 @@
         <v>0</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R36" s="18">
         <f>iferror(lookup(if(Q36="",H36,Q36),{0,1,10,25,100,250,500,1000,5000},{0.0,1.01,0.901,0.8548,0.7021,0.65636,0.58004,0.504,0.504}),"")</f>
@@ -10467,10 +10526,10 @@
         <v>0</v>
       </c>
       <c r="T36" s="19" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="U36" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W36" s="18">
         <f>iferror(USD_GBP*lookup(if(V36="",H36,V36),{0,1,5,10,100,500,1000,2500,5000},{0.0,0.986,1.09,0.835,0.566,0.536,0.417,0.404,0.388}),"")</f>
@@ -10481,10 +10540,10 @@
         <v>0</v>
       </c>
       <c r="Y36" s="19" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="AE36" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG36" s="18">
         <f>iferror(lookup(if(AF36="",H36,AF36),{0,1,10,50,100,1000,10000},{0.0,1.0,0.901,0.855,0.703,0.458,0.403}),"")</f>
@@ -10495,10 +10554,10 @@
         <v>0</v>
       </c>
       <c r="AI36" s="19" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="AJ36" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL36" s="18">
         <f>iferror(lookup(if(AK36="",H36,AK36),{0,1,5,10,100,500,1000,2500,5000,10000,20000,30000,40000,50000,500000},{0.0,1.19,1.19,1.01,0.684,0.648,0.504,0.489,0.391,0.386,0.381,0.376,0.37,0.365,0.36}),"")</f>
@@ -10509,30 +10568,30 @@
         <v>0</v>
       </c>
       <c r="AN36" s="19" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:50">
       <c r="A37" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C37" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="H37" s="17">
         <f>BoardQty*1</f>
@@ -10547,7 +10606,7 @@
         <v>0</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R37" s="18">
         <f>iferror(lookup(if(Q37="",H37,Q37),{0,1,3000},{0.0,0.15015,0.15015}),"")</f>
@@ -10558,10 +10617,10 @@
         <v>0</v>
       </c>
       <c r="T37" s="19" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="U37" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W37" s="18">
         <f>iferror(USD_GBP*lookup(if(V37="",H37,V37),{0,1,3000},{0.0,0.0746,0.0746}),"")</f>
@@ -10572,10 +10631,10 @@
         <v>0</v>
       </c>
       <c r="Y37" s="19" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="AE37" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG37" s="18">
         <f>iferror(lookup(if(AF37="",H37,AF37),{0,1,10,50,100,1000,10000},{0.0,0.53,0.428,0.428,0.264,0.164,0.15}),"")</f>
@@ -10586,10 +10645,10 @@
         <v>0</v>
       </c>
       <c r="AI37" s="19" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="AJ37" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL37" s="18">
         <f>iferror(lookup(if(AK37="",H37,AK37),{0,1,3000},{0.0,0.119,0.119}),"")</f>
@@ -10600,30 +10659,30 @@
         <v>0</v>
       </c>
       <c r="AN37" s="19" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:50">
       <c r="A38" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C38" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="17" t="s">
         <v>162</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="H38" s="17">
         <f>BoardQty*1</f>
@@ -10649,7 +10708,7 @@
         <v>0</v>
       </c>
       <c r="T38" s="19" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="U38" s="17">
         <v>1444</v>
@@ -10663,7 +10722,7 @@
         <v>0</v>
       </c>
       <c r="Y38" s="19" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="AE38" s="17">
         <v>4209</v>
@@ -10677,7 +10736,7 @@
         <v>0</v>
       </c>
       <c r="AI38" s="19" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="AJ38" s="17">
         <v>1444</v>
@@ -10691,7 +10750,7 @@
         <v>0</v>
       </c>
       <c r="AN38" s="19" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="AO38" s="17">
         <v>2960</v>
@@ -10705,30 +10764,30 @@
         <v>0</v>
       </c>
       <c r="AS38" s="19" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:50">
       <c r="A39" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C39" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G39" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="H39" s="17">
         <f>BoardQty*1</f>
@@ -10754,7 +10813,7 @@
         <v>0</v>
       </c>
       <c r="T39" s="19" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="U39" s="17">
         <v>10</v>
@@ -10768,7 +10827,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="19" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="AE39" s="17">
         <v>1300</v>
@@ -10782,10 +10841,10 @@
         <v>0</v>
       </c>
       <c r="AI39" s="19" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="AJ39" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL39" s="18">
         <f>iferror(lookup(if(AK39="",H39,AK39),{0,1,3000},{0.0,0.124,0.124}),"")</f>
@@ -10796,27 +10855,27 @@
         <v>0</v>
       </c>
       <c r="AN39" s="19" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
     </row>
     <row r="40" spans="1:50">
       <c r="A40" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C40" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>169</v>
       </c>
       <c r="H40" s="17">
         <f>BoardQty*1</f>
@@ -10833,22 +10892,22 @@
     </row>
     <row r="41" spans="1:50">
       <c r="A41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F41" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C41" s="17" t="s">
+      <c r="G41" s="17" t="s">
         <v>175</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="H41" s="17">
         <f>BoardQty*1</f>
@@ -10863,7 +10922,7 @@
         <v>0</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R41" s="18">
         <f>iferror(lookup(if(Q41="",H41,Q41),{0,1,10,25,50,100,250,500,1000,5000},{0.0,1.72,1.566,1.5232,1.5154,1.3547,1.35072,1.33034,1.27387,1.18601}),"")</f>
@@ -10874,27 +10933,27 @@
         <v>0</v>
       </c>
       <c r="T41" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:50">
       <c r="A42" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H42" s="17">
         <f>BoardQty*1</f>
@@ -10909,7 +10968,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R42" s="18">
         <f>iferror(lookup(if(Q42="",H42,Q42),{0,1,5000},{0.0,3.63,3.49965}),"")</f>
@@ -10920,10 +10979,10 @@
         <v>0</v>
       </c>
       <c r="T42" s="19" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="U42" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W42" s="18">
         <f>iferror(USD_GBP*lookup(if(V42="",H42,V42),{0,1,10,25,50,100},{0.0,3.61,2.74,2.69,2.64,2.59}),"")</f>
@@ -10934,10 +10993,10 @@
         <v>0</v>
       </c>
       <c r="Y42" s="19" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="AE42" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG42" s="18">
         <f>iferror(lookup(if(AF42="",H42,AF42),{0,1,10,50,100,1000,10000},{0.0,3.58,3.22,3.04,2.64,2.59,2.54}),"")</f>
@@ -10948,10 +11007,10 @@
         <v>0</v>
       </c>
       <c r="AI42" s="19" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="AJ42" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL42" s="18">
         <f>iferror(lookup(if(AK42="",H42,AK42),{0,1,10,5000},{0.0,3.53,3.45,3.33}),"")</f>
@@ -10962,27 +11021,27 @@
         <v>0</v>
       </c>
       <c r="AN42" s="19" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" spans="1:50">
       <c r="A43" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C43" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" s="17" t="s">
         <v>185</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="H43" s="17">
         <f>BoardQty*1</f>
@@ -11008,7 +11067,7 @@
         <v>0</v>
       </c>
       <c r="T43" s="19" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="U43" s="17">
         <v>3893</v>
@@ -11022,7 +11081,7 @@
         <v>0</v>
       </c>
       <c r="Y43" s="19" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="Z43" s="17">
         <v>452</v>
@@ -11036,7 +11095,7 @@
         <v>0</v>
       </c>
       <c r="AD43" s="19" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AE43" s="17">
         <v>506</v>
@@ -11050,7 +11109,7 @@
         <v>0</v>
       </c>
       <c r="AI43" s="19" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="AJ43" s="17">
         <v>100</v>
@@ -11064,27 +11123,27 @@
         <v>0</v>
       </c>
       <c r="AN43" s="19" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="44" spans="1:50">
       <c r="A44" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H44" s="17">
         <f>BoardQty*1</f>
@@ -11110,7 +11169,7 @@
         <v>0</v>
       </c>
       <c r="T44" s="19" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="U44" s="17">
         <v>3487</v>
@@ -11124,7 +11183,7 @@
         <v>0</v>
       </c>
       <c r="Y44" s="19" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="AE44" s="17">
         <v>4611</v>
@@ -11138,7 +11197,7 @@
         <v>0</v>
       </c>
       <c r="AI44" s="19" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="AJ44" s="17">
         <v>3487</v>
@@ -11152,27 +11211,27 @@
         <v>0</v>
       </c>
       <c r="AN44" s="19" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
     </row>
     <row r="45" spans="1:50">
       <c r="A45" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="G45" s="17" t="s">
         <v>194</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="H45" s="17">
         <f>BoardQty*1</f>
@@ -11187,7 +11246,7 @@
         <v>0</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R45" s="18">
         <f>iferror(lookup(if(Q45="",H45,Q45),{0,1,168},{0.0,13.46006,13.46006}),"")</f>
@@ -11198,27 +11257,27 @@
         <v>0</v>
       </c>
       <c r="T45" s="19" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="1:50">
       <c r="A46" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C46" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="G46" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>198</v>
       </c>
       <c r="H46" s="17">
         <f>BoardQty*1</f>
@@ -11233,7 +11292,7 @@
         <v>0</v>
       </c>
       <c r="P46" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R46" s="18">
         <f>iferror(lookup(if(Q46="",H46,Q46),{0,1,25,100},{0.0,2.39,1.99,1.81}),"")</f>
@@ -11244,10 +11303,10 @@
         <v>0</v>
       </c>
       <c r="T46" s="19" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AE46" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AG46" s="18">
         <f>iferror(lookup(if(AF46="",H46,AF46),{0,1,10,50,100,1000,10000},{0.0,2.39,2.39,1.99,1.81,1.81,1.81}),"")</f>
@@ -11258,10 +11317,10 @@
         <v>0</v>
       </c>
       <c r="AI46" s="19" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="AJ46" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL46" s="18">
         <f>iferror(lookup(if(AK46="",H46,AK46),{0,1,220},{0.0,1.81,1.81}),"")</f>
@@ -11272,27 +11331,27 @@
         <v>0</v>
       </c>
       <c r="AN46" s="19" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
     </row>
     <row r="47" spans="1:50">
       <c r="A47" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H47" s="17">
         <f>BoardQty*1</f>
@@ -11318,10 +11377,10 @@
         <v>0</v>
       </c>
       <c r="T47" s="19" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="U47" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W47" s="18">
         <f>iferror(USD_GBP*lookup(if(V47="",H47,V47),{0,1,5,10,100,150,500,3000},{0.0,0.795,0.795,0.65,0.398,0.398,0.28,0.268}),"")</f>
@@ -11332,7 +11391,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="19" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="Z47" s="17">
         <v>6</v>
@@ -11346,7 +11405,7 @@
         <v>0</v>
       </c>
       <c r="AD47" s="19" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="AE47" s="17">
         <v>2920</v>
@@ -11360,10 +11419,10 @@
         <v>0</v>
       </c>
       <c r="AI47" s="19" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="AJ47" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL47" s="18">
         <f>iferror(lookup(if(AK47="",H47,AK47),{0,1,5,10,100,3000,9000,24000,45000},{0.0,0.85,0.85,0.71,0.458,0.238,0.233,0.216,0.21}),"")</f>
@@ -11374,27 +11433,27 @@
         <v>0</v>
       </c>
       <c r="AN47" s="19" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
     </row>
     <row r="48" spans="1:50">
       <c r="A48" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H48" s="17">
         <f>BoardQty*1</f>
@@ -11420,10 +11479,10 @@
         <v>0</v>
       </c>
       <c r="T48" s="19" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="U48" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="W48" s="18">
         <f>iferror(USD_GBP*lookup(if(V48="",H48,V48),{0,1,3000},{0.0,0.25,0.25}),"")</f>
@@ -11434,7 +11493,7 @@
         <v>0</v>
       </c>
       <c r="Y48" s="19" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AE48" s="17">
         <v>982</v>
@@ -11448,10 +11507,10 @@
         <v>0</v>
       </c>
       <c r="AI48" s="19" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="AJ48" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL48" s="18">
         <f>iferror(lookup(if(AK48="",H48,AK48),{0,1,3000,6000,12000,18000,24000,30000,300000},{0.0,0.34,0.34,0.335,0.33,0.326,0.322,0.317,0.313}),"")</f>
@@ -11462,27 +11521,27 @@
         <v>0</v>
       </c>
       <c r="AN48" s="19" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
     </row>
     <row r="49" spans="1:49">
       <c r="A49" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F49" s="17" t="s">
         <v>15</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H49" s="17">
         <f>BoardQty*1</f>
@@ -11508,7 +11567,7 @@
         <v>0</v>
       </c>
       <c r="T49" s="19" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="U49" s="17">
         <v>490</v>
@@ -11522,7 +11581,7 @@
         <v>0</v>
       </c>
       <c r="Y49" s="19" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AE49" s="17">
         <v>13</v>
@@ -11536,7 +11595,7 @@
         <v>0</v>
       </c>
       <c r="AI49" s="19" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="AJ49" s="17">
         <v>490</v>
@@ -11550,27 +11609,27 @@
         <v>0</v>
       </c>
       <c r="AN49" s="19" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
     </row>
     <row r="50" spans="1:49">
       <c r="A50" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" s="17" t="s">
         <v>216</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>215</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>15</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H50" s="17">
         <f>BoardQty*1</f>
@@ -11596,7 +11655,7 @@
         <v>0</v>
       </c>
       <c r="T50" s="19" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="U50" s="17">
         <v>500</v>
@@ -11610,7 +11669,7 @@
         <v>0</v>
       </c>
       <c r="Y50" s="19" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="AE50" s="17">
         <v>475</v>
@@ -11624,7 +11683,7 @@
         <v>0</v>
       </c>
       <c r="AI50" s="19" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="AJ50" s="17">
         <v>500</v>
@@ -11638,27 +11697,27 @@
         <v>0</v>
       </c>
       <c r="AN50" s="19" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:49">
       <c r="A51" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C51" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="G51" s="17" t="s">
         <v>221</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>220</v>
       </c>
       <c r="H51" s="17">
         <f>BoardQty*4</f>
@@ -11673,7 +11732,7 @@
         <v>0</v>
       </c>
       <c r="P51" s="20" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R51" s="18">
         <f>iferror(lookup(if(Q51="",H51,Q51),{0,1,2000},{0.0,1.336,1.336}),"")</f>
@@ -11684,7 +11743,7 @@
         <v>0</v>
       </c>
       <c r="T51" s="19" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="Z51" s="17">
         <v>1990</v>
@@ -11698,7 +11757,7 @@
         <v>0</v>
       </c>
       <c r="AD51" s="19" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="AE51" s="17">
         <v>594</v>
@@ -11712,22 +11771,22 @@
         <v>0</v>
       </c>
       <c r="AI51" s="19" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:49">
       <c r="B53" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J53" s="5">
         <f>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(arrow_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(tme_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(lcsc_part_data)+3)))</f>
         <v>0</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L53" s="6">
         <f>IFERROR(IF(OR(L7:L51),COUNTIFS(L7:L51,"&gt;0",N7:N51,"&lt;&gt;")&amp;" of "&amp;(ROWS(N7:N51)-COUNTBLANK(N7:N51))&amp;" parts purchased",""),"")</f>
@@ -11738,7 +11797,7 @@
         <v>0</v>
       </c>
       <c r="P53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Q53" s="6">
         <f>IFERROR(IF(OR(Q7:Q51),COUNTIFS(Q7:Q51,"&gt;0",S7:S51,"&lt;&gt;")&amp;" of "&amp;(ROWS(S7:S51)-COUNTBLANK(S7:S51))&amp;" parts purchased",""),"")</f>
@@ -11749,7 +11808,7 @@
         <v>0</v>
       </c>
       <c r="U53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="V53" s="6">
         <f>IFERROR(IF(OR(V7:V51),COUNTIFS(V7:V51,"&gt;0",X7:X51,"&lt;&gt;")&amp;" of "&amp;(ROWS(X7:X51)-COUNTBLANK(X7:X51))&amp;" parts purchased",""),"")</f>
@@ -11760,7 +11819,7 @@
         <v>0</v>
       </c>
       <c r="Z53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AA53" s="6">
         <f>IFERROR(IF(OR(AA7:AA51),COUNTIFS(AA7:AA51,"&gt;0",AC7:AC51,"&lt;&gt;")&amp;" of "&amp;(ROWS(AC7:AC51)-COUNTBLANK(AC7:AC51))&amp;" parts purchased",""),"")</f>
@@ -11771,7 +11830,7 @@
         <v>0</v>
       </c>
       <c r="AE53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AF53" s="6">
         <f>IFERROR(IF(OR(AF7:AF51),COUNTIFS(AF7:AF51,"&gt;0",AH7:AH51,"&lt;&gt;")&amp;" of "&amp;(ROWS(AH7:AH51)-COUNTBLANK(AH7:AH51))&amp;" parts purchased",""),"")</f>
@@ -11782,7 +11841,7 @@
         <v>0</v>
       </c>
       <c r="AJ53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AK53" s="6">
         <f>IFERROR(IF(OR(AK7:AK51),COUNTIFS(AK7:AK51,"&gt;0",AM7:AM51,"&lt;&gt;")&amp;" of "&amp;(ROWS(AM7:AM51)-COUNTBLANK(AM7:AM51))&amp;" parts purchased",""),"")</f>
@@ -11793,7 +11852,7 @@
         <v>0</v>
       </c>
       <c r="AO53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AP53" s="6">
         <f>IFERROR(IF(OR(AP7:AP51),COUNTIFS(AP7:AP51,"&gt;0",AR7:AR51,"&lt;&gt;")&amp;" of "&amp;(ROWS(AR7:AR51)-COUNTBLANK(AR7:AR51))&amp;" parts purchased",""),"")</f>
@@ -11804,7 +11863,7 @@
         <v>0</v>
       </c>
       <c r="AT53" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AU53" s="6">
         <f>IFERROR(IF(OR(AU7:AU51),COUNTIFS(AU7:AU51,"&gt;0",AW7:AW51,"&lt;&gt;")&amp;" of "&amp;(ROWS(AW7:AW51)-COUNTBLANK(AW7:AW51))&amp;" parts purchased",""),"")</f>
@@ -11817,13 +11876,13 @@
     </row>
     <row r="54" spans="1:49">
       <c r="B54" s="21" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C54">
         <v>1.293904700565222</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L54">
         <f t="array" ref="L54">IFERROR(CONCATENATE(INDEX(O7:O51,SMALL(IF(ISNUMBER(L7:L51),IF(L7:L51&gt;0,IF(O7:O51&lt;&gt;"",ROW(L7:L51)-MIN(ROW(L7:L51))+1))),ROW()-ROW(A$54)+1)),",",TEXT(INDEX(L7:L51,SMALL(IF(ISNUMBER(L7:L51),IF(L7:L51&gt;0,IF(O7:O51&lt;&gt;"",ROW(L7:L51)-MIN(ROW(L7:L51))+1))),ROW()-ROW(A$54)+1)),"##0"),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A51,SMALL(IF(ISNUMBER(L7:L51),IF(L7:L51&gt;0,IF(O7:O51&lt;&gt;"",ROW(L7:L51)-MIN(ROW(L7:L51))+1))),ROW()-ROW(A$54)+1)),",",";")),"")</f>
@@ -11910,7 +11969,7 @@
     </row>
     <row r="56" spans="1:49">
       <c r="A56" s="2" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="L56">
         <f t="array" ref="L56">IFERROR(CONCATENATE(INDEX(O7:O51,SMALL(IF(ISNUMBER(L7:L51),IF(L7:L51&gt;0,IF(O7:O51&lt;&gt;"",ROW(L7:L51)-MIN(ROW(L7:L51))+1))),ROW()-ROW(A$54)+1)),",",TEXT(INDEX(L7:L51,SMALL(IF(ISNUMBER(L7:L51),IF(L7:L51&gt;0,IF(O7:O51&lt;&gt;"",ROW(L7:L51)-MIN(ROW(L7:L51))+1))),ROW()-ROW(A$54)+1)),"##0"),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A51,SMALL(IF(ISNUMBER(L7:L51),IF(L7:L51&gt;0,IF(O7:O51&lt;&gt;"",ROW(L7:L51)-MIN(ROW(L7:L51))+1))),ROW()-ROW(A$54)+1)),",",";")),"")</f>
@@ -15767,7 +15826,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="AP13">
     <cfRule type="expression" dxfId="3" priority="1062">
-      <formula>AND(AP13&gt;0,AP13&lt;15000)</formula>
+      <formula>AND(AP13&gt;0,AP13&lt;200)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1063" operator="greaterThan">
       <formula>AO13</formula>
@@ -15963,78 +16022,104 @@
       <formula>J7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AT19">
+  <conditionalFormatting sqref="AT13">
     <cfRule type="cellIs" dxfId="1" priority="1120" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="1121" operator="lessThan">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT19">
+    <cfRule type="cellIs" dxfId="1" priority="1126" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1127" operator="lessThan">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT20">
-    <cfRule type="cellIs" dxfId="1" priority="1125" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1126" operator="lessThan">
-      <formula>H20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT35">
     <cfRule type="cellIs" dxfId="1" priority="1131" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="1132" operator="lessThan">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT35">
+    <cfRule type="cellIs" dxfId="1" priority="1137" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1138" operator="lessThan">
       <formula>H35</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AU13">
+    <cfRule type="expression" dxfId="3" priority="1122">
+      <formula>AND(AU13&gt;0,AU13&lt;100)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1123" operator="greaterThan">
+      <formula>AT13</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AU19">
-    <cfRule type="cellIs" dxfId="1" priority="1122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1128" operator="greaterThan">
       <formula>AT19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU20">
-    <cfRule type="expression" dxfId="3" priority="1127">
+    <cfRule type="expression" dxfId="3" priority="1133">
       <formula>AND(AU20&gt;0,AU20&lt;50)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1134" operator="greaterThan">
       <formula>AT20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU35">
-    <cfRule type="expression" dxfId="3" priority="1133">
+    <cfRule type="expression" dxfId="3" priority="1139">
       <formula>AND(AU35&gt;0,AU35&lt;5)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1140" operator="greaterThan">
       <formula>AT35</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AV13">
+    <cfRule type="cellIs" dxfId="4" priority="1125" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AV19">
+    <cfRule type="cellIs" dxfId="4" priority="1130" operator="lessThanOrEqual">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV20">
+    <cfRule type="cellIs" dxfId="4" priority="1136" operator="lessThanOrEqual">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV35">
+    <cfRule type="cellIs" dxfId="4" priority="1142" operator="lessThanOrEqual">
+      <formula>I35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW13">
     <cfRule type="cellIs" dxfId="4" priority="1124" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV20">
-    <cfRule type="cellIs" dxfId="4" priority="1130" operator="lessThanOrEqual">
-      <formula>I20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV35">
-    <cfRule type="cellIs" dxfId="4" priority="1136" operator="lessThanOrEqual">
-      <formula>I35</formula>
+      <formula>J13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW19">
-    <cfRule type="cellIs" dxfId="4" priority="1123" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1129" operator="lessThanOrEqual">
       <formula>J19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW20">
-    <cfRule type="cellIs" dxfId="4" priority="1129" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1135" operator="lessThanOrEqual">
       <formula>J20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW35">
-    <cfRule type="cellIs" dxfId="4" priority="1135" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1141" operator="lessThanOrEqual">
       <formula>J35</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18683,198 +18768,199 @@
     <hyperlink ref="AI13" r:id="rId39"/>
     <hyperlink ref="AN13" r:id="rId40"/>
     <hyperlink ref="AS13" r:id="rId41"/>
-    <hyperlink ref="G14" r:id="rId42"/>
-    <hyperlink ref="T14" r:id="rId43"/>
-    <hyperlink ref="Y14" r:id="rId44"/>
-    <hyperlink ref="AD14" r:id="rId45"/>
-    <hyperlink ref="AI14" r:id="rId46"/>
-    <hyperlink ref="AN14" r:id="rId47"/>
-    <hyperlink ref="G15" r:id="rId48"/>
-    <hyperlink ref="T15" r:id="rId49"/>
-    <hyperlink ref="Y15" r:id="rId50"/>
-    <hyperlink ref="AI15" r:id="rId51"/>
-    <hyperlink ref="AN15" r:id="rId52"/>
-    <hyperlink ref="G16" r:id="rId53"/>
-    <hyperlink ref="T16" r:id="rId54"/>
-    <hyperlink ref="AI16" r:id="rId55"/>
-    <hyperlink ref="AN16" r:id="rId56"/>
-    <hyperlink ref="AS16" r:id="rId57"/>
-    <hyperlink ref="G17" r:id="rId58"/>
-    <hyperlink ref="T17" r:id="rId59"/>
-    <hyperlink ref="AI17" r:id="rId60"/>
-    <hyperlink ref="AS17" r:id="rId61"/>
-    <hyperlink ref="G18" r:id="rId62"/>
-    <hyperlink ref="T18" r:id="rId63"/>
-    <hyperlink ref="Y18" r:id="rId64"/>
-    <hyperlink ref="AI18" r:id="rId65"/>
-    <hyperlink ref="AN18" r:id="rId66"/>
-    <hyperlink ref="G19" r:id="rId67"/>
-    <hyperlink ref="T19" r:id="rId68"/>
-    <hyperlink ref="Y19" r:id="rId69"/>
-    <hyperlink ref="AI19" r:id="rId70"/>
-    <hyperlink ref="AN19" r:id="rId71"/>
-    <hyperlink ref="AX19" r:id="rId72"/>
-    <hyperlink ref="G20" r:id="rId73"/>
-    <hyperlink ref="T20" r:id="rId74"/>
-    <hyperlink ref="Y20" r:id="rId75"/>
-    <hyperlink ref="AD20" r:id="rId76"/>
-    <hyperlink ref="AI20" r:id="rId77"/>
-    <hyperlink ref="AN20" r:id="rId78"/>
-    <hyperlink ref="AS20" r:id="rId79"/>
-    <hyperlink ref="AX20" r:id="rId80"/>
-    <hyperlink ref="G21" r:id="rId81"/>
-    <hyperlink ref="T21" r:id="rId82"/>
-    <hyperlink ref="AI21" r:id="rId83"/>
-    <hyperlink ref="G22" r:id="rId84"/>
-    <hyperlink ref="T22" r:id="rId85"/>
-    <hyperlink ref="G23" r:id="rId86"/>
-    <hyperlink ref="T23" r:id="rId87"/>
-    <hyperlink ref="G24" r:id="rId88"/>
-    <hyperlink ref="T24" r:id="rId89"/>
-    <hyperlink ref="G25" r:id="rId90"/>
-    <hyperlink ref="T25" r:id="rId91"/>
-    <hyperlink ref="AI25" r:id="rId92"/>
-    <hyperlink ref="G26" r:id="rId93"/>
-    <hyperlink ref="T26" r:id="rId94"/>
-    <hyperlink ref="Y26" r:id="rId95"/>
-    <hyperlink ref="AI26" r:id="rId96"/>
-    <hyperlink ref="AN26" r:id="rId97"/>
-    <hyperlink ref="AS26" r:id="rId98"/>
-    <hyperlink ref="G27" r:id="rId99"/>
-    <hyperlink ref="T27" r:id="rId100"/>
-    <hyperlink ref="Y27" r:id="rId101"/>
-    <hyperlink ref="AI27" r:id="rId102"/>
-    <hyperlink ref="AN27" r:id="rId103"/>
-    <hyperlink ref="AS27" r:id="rId104"/>
-    <hyperlink ref="G28" r:id="rId105"/>
-    <hyperlink ref="T28" r:id="rId106"/>
-    <hyperlink ref="Y28" r:id="rId107"/>
-    <hyperlink ref="AI28" r:id="rId108"/>
-    <hyperlink ref="G29" r:id="rId109"/>
-    <hyperlink ref="T29" r:id="rId110"/>
-    <hyperlink ref="Y29" r:id="rId111"/>
-    <hyperlink ref="AI29" r:id="rId112"/>
-    <hyperlink ref="AN29" r:id="rId113"/>
-    <hyperlink ref="AS29" r:id="rId114"/>
-    <hyperlink ref="G30" r:id="rId115"/>
-    <hyperlink ref="T30" r:id="rId116"/>
-    <hyperlink ref="Y30" r:id="rId117"/>
-    <hyperlink ref="AD30" r:id="rId118"/>
-    <hyperlink ref="AI30" r:id="rId119"/>
-    <hyperlink ref="AN30" r:id="rId120"/>
-    <hyperlink ref="G31" r:id="rId121"/>
-    <hyperlink ref="T31" r:id="rId122"/>
-    <hyperlink ref="Y31" r:id="rId123"/>
-    <hyperlink ref="AI31" r:id="rId124"/>
-    <hyperlink ref="AN31" r:id="rId125"/>
-    <hyperlink ref="G32" r:id="rId126"/>
-    <hyperlink ref="T32" r:id="rId127"/>
-    <hyperlink ref="Y32" r:id="rId128"/>
-    <hyperlink ref="AD32" r:id="rId129"/>
-    <hyperlink ref="AI32" r:id="rId130"/>
-    <hyperlink ref="AN32" r:id="rId131"/>
-    <hyperlink ref="AS32" r:id="rId132"/>
-    <hyperlink ref="G33" r:id="rId133"/>
-    <hyperlink ref="T33" r:id="rId134"/>
-    <hyperlink ref="Y33" r:id="rId135"/>
-    <hyperlink ref="AD33" r:id="rId136"/>
-    <hyperlink ref="AI33" r:id="rId137"/>
-    <hyperlink ref="AN33" r:id="rId138"/>
-    <hyperlink ref="AS33" r:id="rId139"/>
-    <hyperlink ref="G34" r:id="rId140"/>
-    <hyperlink ref="T34" r:id="rId141"/>
-    <hyperlink ref="Y34" r:id="rId142"/>
-    <hyperlink ref="AD34" r:id="rId143"/>
-    <hyperlink ref="AI34" r:id="rId144"/>
-    <hyperlink ref="AN34" r:id="rId145"/>
-    <hyperlink ref="G35" r:id="rId146"/>
-    <hyperlink ref="T35" r:id="rId147"/>
-    <hyperlink ref="Y35" r:id="rId148"/>
-    <hyperlink ref="AD35" r:id="rId149"/>
-    <hyperlink ref="AI35" r:id="rId150"/>
-    <hyperlink ref="AN35" r:id="rId151"/>
-    <hyperlink ref="AX35" r:id="rId152"/>
-    <hyperlink ref="G36" r:id="rId153"/>
-    <hyperlink ref="T36" r:id="rId154"/>
-    <hyperlink ref="Y36" r:id="rId155"/>
-    <hyperlink ref="AI36" r:id="rId156"/>
-    <hyperlink ref="AN36" r:id="rId157"/>
-    <hyperlink ref="G37" r:id="rId158"/>
-    <hyperlink ref="T37" r:id="rId159"/>
-    <hyperlink ref="Y37" r:id="rId160"/>
-    <hyperlink ref="AI37" r:id="rId161"/>
-    <hyperlink ref="AN37" r:id="rId162"/>
-    <hyperlink ref="G38" r:id="rId163"/>
-    <hyperlink ref="T38" r:id="rId164"/>
-    <hyperlink ref="Y38" r:id="rId165"/>
-    <hyperlink ref="AI38" r:id="rId166"/>
-    <hyperlink ref="AN38" r:id="rId167"/>
-    <hyperlink ref="AS38" r:id="rId168"/>
-    <hyperlink ref="G39" r:id="rId169"/>
-    <hyperlink ref="T39" r:id="rId170"/>
-    <hyperlink ref="Y39" r:id="rId171"/>
-    <hyperlink ref="AI39" r:id="rId172"/>
-    <hyperlink ref="AN39" r:id="rId173"/>
-    <hyperlink ref="G40" r:id="rId174"/>
-    <hyperlink ref="G41" r:id="rId175"/>
-    <hyperlink ref="T41" r:id="rId176"/>
-    <hyperlink ref="G42" r:id="rId177"/>
-    <hyperlink ref="T42" r:id="rId178"/>
-    <hyperlink ref="Y42" r:id="rId179"/>
-    <hyperlink ref="AI42" r:id="rId180"/>
-    <hyperlink ref="AN42" r:id="rId181"/>
-    <hyperlink ref="G43" r:id="rId182"/>
-    <hyperlink ref="T43" r:id="rId183"/>
-    <hyperlink ref="Y43" r:id="rId184"/>
-    <hyperlink ref="AD43" r:id="rId185"/>
-    <hyperlink ref="AI43" r:id="rId186"/>
-    <hyperlink ref="AN43" r:id="rId187"/>
-    <hyperlink ref="G44" r:id="rId188"/>
-    <hyperlink ref="T44" r:id="rId189"/>
-    <hyperlink ref="Y44" r:id="rId190"/>
-    <hyperlink ref="AI44" r:id="rId191"/>
-    <hyperlink ref="AN44" r:id="rId192"/>
-    <hyperlink ref="G45" r:id="rId193"/>
-    <hyperlink ref="T45" r:id="rId194"/>
-    <hyperlink ref="G46" r:id="rId195"/>
-    <hyperlink ref="T46" r:id="rId196"/>
-    <hyperlink ref="AI46" r:id="rId197"/>
-    <hyperlink ref="AN46" r:id="rId198"/>
-    <hyperlink ref="G47" r:id="rId199"/>
-    <hyperlink ref="T47" r:id="rId200"/>
-    <hyperlink ref="Y47" r:id="rId201"/>
-    <hyperlink ref="AD47" r:id="rId202"/>
-    <hyperlink ref="AI47" r:id="rId203"/>
-    <hyperlink ref="AN47" r:id="rId204"/>
-    <hyperlink ref="G48" r:id="rId205"/>
-    <hyperlink ref="T48" r:id="rId206"/>
-    <hyperlink ref="Y48" r:id="rId207"/>
-    <hyperlink ref="AI48" r:id="rId208"/>
-    <hyperlink ref="AN48" r:id="rId209"/>
-    <hyperlink ref="G49" r:id="rId210"/>
-    <hyperlink ref="T49" r:id="rId211"/>
-    <hyperlink ref="Y49" r:id="rId212"/>
-    <hyperlink ref="AI49" r:id="rId213"/>
-    <hyperlink ref="AN49" r:id="rId214"/>
-    <hyperlink ref="G50" r:id="rId215"/>
-    <hyperlink ref="T50" r:id="rId216"/>
-    <hyperlink ref="Y50" r:id="rId217"/>
-    <hyperlink ref="AI50" r:id="rId218"/>
-    <hyperlink ref="AN50" r:id="rId219"/>
-    <hyperlink ref="G51" r:id="rId220"/>
-    <hyperlink ref="T51" r:id="rId221"/>
-    <hyperlink ref="AD51" r:id="rId222"/>
-    <hyperlink ref="AI51" r:id="rId223"/>
-    <hyperlink ref="K53" r:id="rId224"/>
-    <hyperlink ref="P53" r:id="rId225"/>
-    <hyperlink ref="U53" r:id="rId226"/>
-    <hyperlink ref="Z53" r:id="rId227"/>
-    <hyperlink ref="AE53" r:id="rId228"/>
-    <hyperlink ref="AJ53" r:id="rId229"/>
-    <hyperlink ref="AO53" r:id="rId230"/>
-    <hyperlink ref="AT53" r:id="rId231"/>
+    <hyperlink ref="AX13" r:id="rId42"/>
+    <hyperlink ref="G14" r:id="rId43"/>
+    <hyperlink ref="T14" r:id="rId44"/>
+    <hyperlink ref="Y14" r:id="rId45"/>
+    <hyperlink ref="AD14" r:id="rId46"/>
+    <hyperlink ref="AI14" r:id="rId47"/>
+    <hyperlink ref="AN14" r:id="rId48"/>
+    <hyperlink ref="G15" r:id="rId49"/>
+    <hyperlink ref="T15" r:id="rId50"/>
+    <hyperlink ref="Y15" r:id="rId51"/>
+    <hyperlink ref="AI15" r:id="rId52"/>
+    <hyperlink ref="AN15" r:id="rId53"/>
+    <hyperlink ref="G16" r:id="rId54"/>
+    <hyperlink ref="T16" r:id="rId55"/>
+    <hyperlink ref="AI16" r:id="rId56"/>
+    <hyperlink ref="AN16" r:id="rId57"/>
+    <hyperlink ref="AS16" r:id="rId58"/>
+    <hyperlink ref="G17" r:id="rId59"/>
+    <hyperlink ref="T17" r:id="rId60"/>
+    <hyperlink ref="AI17" r:id="rId61"/>
+    <hyperlink ref="AS17" r:id="rId62"/>
+    <hyperlink ref="G18" r:id="rId63"/>
+    <hyperlink ref="T18" r:id="rId64"/>
+    <hyperlink ref="Y18" r:id="rId65"/>
+    <hyperlink ref="AI18" r:id="rId66"/>
+    <hyperlink ref="AN18" r:id="rId67"/>
+    <hyperlink ref="G19" r:id="rId68"/>
+    <hyperlink ref="T19" r:id="rId69"/>
+    <hyperlink ref="Y19" r:id="rId70"/>
+    <hyperlink ref="AI19" r:id="rId71"/>
+    <hyperlink ref="AN19" r:id="rId72"/>
+    <hyperlink ref="AX19" r:id="rId73"/>
+    <hyperlink ref="G20" r:id="rId74"/>
+    <hyperlink ref="T20" r:id="rId75"/>
+    <hyperlink ref="Y20" r:id="rId76"/>
+    <hyperlink ref="AD20" r:id="rId77"/>
+    <hyperlink ref="AI20" r:id="rId78"/>
+    <hyperlink ref="AN20" r:id="rId79"/>
+    <hyperlink ref="AS20" r:id="rId80"/>
+    <hyperlink ref="AX20" r:id="rId81"/>
+    <hyperlink ref="G21" r:id="rId82"/>
+    <hyperlink ref="T21" r:id="rId83"/>
+    <hyperlink ref="AI21" r:id="rId84"/>
+    <hyperlink ref="G22" r:id="rId85"/>
+    <hyperlink ref="T22" r:id="rId86"/>
+    <hyperlink ref="G23" r:id="rId87"/>
+    <hyperlink ref="T23" r:id="rId88"/>
+    <hyperlink ref="G24" r:id="rId89"/>
+    <hyperlink ref="T24" r:id="rId90"/>
+    <hyperlink ref="G25" r:id="rId91"/>
+    <hyperlink ref="T25" r:id="rId92"/>
+    <hyperlink ref="AI25" r:id="rId93"/>
+    <hyperlink ref="G26" r:id="rId94"/>
+    <hyperlink ref="T26" r:id="rId95"/>
+    <hyperlink ref="Y26" r:id="rId96"/>
+    <hyperlink ref="AI26" r:id="rId97"/>
+    <hyperlink ref="AN26" r:id="rId98"/>
+    <hyperlink ref="AS26" r:id="rId99"/>
+    <hyperlink ref="G27" r:id="rId100"/>
+    <hyperlink ref="T27" r:id="rId101"/>
+    <hyperlink ref="Y27" r:id="rId102"/>
+    <hyperlink ref="AI27" r:id="rId103"/>
+    <hyperlink ref="AN27" r:id="rId104"/>
+    <hyperlink ref="AS27" r:id="rId105"/>
+    <hyperlink ref="G28" r:id="rId106"/>
+    <hyperlink ref="T28" r:id="rId107"/>
+    <hyperlink ref="Y28" r:id="rId108"/>
+    <hyperlink ref="AI28" r:id="rId109"/>
+    <hyperlink ref="G29" r:id="rId110"/>
+    <hyperlink ref="T29" r:id="rId111"/>
+    <hyperlink ref="Y29" r:id="rId112"/>
+    <hyperlink ref="AI29" r:id="rId113"/>
+    <hyperlink ref="AN29" r:id="rId114"/>
+    <hyperlink ref="AS29" r:id="rId115"/>
+    <hyperlink ref="G30" r:id="rId116"/>
+    <hyperlink ref="T30" r:id="rId117"/>
+    <hyperlink ref="Y30" r:id="rId118"/>
+    <hyperlink ref="AD30" r:id="rId119"/>
+    <hyperlink ref="AI30" r:id="rId120"/>
+    <hyperlink ref="AN30" r:id="rId121"/>
+    <hyperlink ref="G31" r:id="rId122"/>
+    <hyperlink ref="T31" r:id="rId123"/>
+    <hyperlink ref="Y31" r:id="rId124"/>
+    <hyperlink ref="AI31" r:id="rId125"/>
+    <hyperlink ref="AN31" r:id="rId126"/>
+    <hyperlink ref="G32" r:id="rId127"/>
+    <hyperlink ref="T32" r:id="rId128"/>
+    <hyperlink ref="Y32" r:id="rId129"/>
+    <hyperlink ref="AD32" r:id="rId130"/>
+    <hyperlink ref="AI32" r:id="rId131"/>
+    <hyperlink ref="AN32" r:id="rId132"/>
+    <hyperlink ref="AS32" r:id="rId133"/>
+    <hyperlink ref="G33" r:id="rId134"/>
+    <hyperlink ref="T33" r:id="rId135"/>
+    <hyperlink ref="Y33" r:id="rId136"/>
+    <hyperlink ref="AD33" r:id="rId137"/>
+    <hyperlink ref="AI33" r:id="rId138"/>
+    <hyperlink ref="AN33" r:id="rId139"/>
+    <hyperlink ref="AS33" r:id="rId140"/>
+    <hyperlink ref="G34" r:id="rId141"/>
+    <hyperlink ref="T34" r:id="rId142"/>
+    <hyperlink ref="Y34" r:id="rId143"/>
+    <hyperlink ref="AD34" r:id="rId144"/>
+    <hyperlink ref="AI34" r:id="rId145"/>
+    <hyperlink ref="AN34" r:id="rId146"/>
+    <hyperlink ref="G35" r:id="rId147"/>
+    <hyperlink ref="T35" r:id="rId148"/>
+    <hyperlink ref="Y35" r:id="rId149"/>
+    <hyperlink ref="AD35" r:id="rId150"/>
+    <hyperlink ref="AI35" r:id="rId151"/>
+    <hyperlink ref="AN35" r:id="rId152"/>
+    <hyperlink ref="AX35" r:id="rId153"/>
+    <hyperlink ref="G36" r:id="rId154"/>
+    <hyperlink ref="T36" r:id="rId155"/>
+    <hyperlink ref="Y36" r:id="rId156"/>
+    <hyperlink ref="AI36" r:id="rId157"/>
+    <hyperlink ref="AN36" r:id="rId158"/>
+    <hyperlink ref="G37" r:id="rId159"/>
+    <hyperlink ref="T37" r:id="rId160"/>
+    <hyperlink ref="Y37" r:id="rId161"/>
+    <hyperlink ref="AI37" r:id="rId162"/>
+    <hyperlink ref="AN37" r:id="rId163"/>
+    <hyperlink ref="G38" r:id="rId164"/>
+    <hyperlink ref="T38" r:id="rId165"/>
+    <hyperlink ref="Y38" r:id="rId166"/>
+    <hyperlink ref="AI38" r:id="rId167"/>
+    <hyperlink ref="AN38" r:id="rId168"/>
+    <hyperlink ref="AS38" r:id="rId169"/>
+    <hyperlink ref="G39" r:id="rId170"/>
+    <hyperlink ref="T39" r:id="rId171"/>
+    <hyperlink ref="Y39" r:id="rId172"/>
+    <hyperlink ref="AI39" r:id="rId173"/>
+    <hyperlink ref="AN39" r:id="rId174"/>
+    <hyperlink ref="G40" r:id="rId175"/>
+    <hyperlink ref="G41" r:id="rId176"/>
+    <hyperlink ref="T41" r:id="rId177"/>
+    <hyperlink ref="G42" r:id="rId178"/>
+    <hyperlink ref="T42" r:id="rId179"/>
+    <hyperlink ref="Y42" r:id="rId180"/>
+    <hyperlink ref="AI42" r:id="rId181"/>
+    <hyperlink ref="AN42" r:id="rId182"/>
+    <hyperlink ref="G43" r:id="rId183"/>
+    <hyperlink ref="T43" r:id="rId184"/>
+    <hyperlink ref="Y43" r:id="rId185"/>
+    <hyperlink ref="AD43" r:id="rId186"/>
+    <hyperlink ref="AI43" r:id="rId187"/>
+    <hyperlink ref="AN43" r:id="rId188"/>
+    <hyperlink ref="G44" r:id="rId189"/>
+    <hyperlink ref="T44" r:id="rId190"/>
+    <hyperlink ref="Y44" r:id="rId191"/>
+    <hyperlink ref="AI44" r:id="rId192"/>
+    <hyperlink ref="AN44" r:id="rId193"/>
+    <hyperlink ref="G45" r:id="rId194"/>
+    <hyperlink ref="T45" r:id="rId195"/>
+    <hyperlink ref="G46" r:id="rId196"/>
+    <hyperlink ref="T46" r:id="rId197"/>
+    <hyperlink ref="AI46" r:id="rId198"/>
+    <hyperlink ref="AN46" r:id="rId199"/>
+    <hyperlink ref="G47" r:id="rId200"/>
+    <hyperlink ref="T47" r:id="rId201"/>
+    <hyperlink ref="Y47" r:id="rId202"/>
+    <hyperlink ref="AD47" r:id="rId203"/>
+    <hyperlink ref="AI47" r:id="rId204"/>
+    <hyperlink ref="AN47" r:id="rId205"/>
+    <hyperlink ref="G48" r:id="rId206"/>
+    <hyperlink ref="T48" r:id="rId207"/>
+    <hyperlink ref="Y48" r:id="rId208"/>
+    <hyperlink ref="AI48" r:id="rId209"/>
+    <hyperlink ref="AN48" r:id="rId210"/>
+    <hyperlink ref="G49" r:id="rId211"/>
+    <hyperlink ref="T49" r:id="rId212"/>
+    <hyperlink ref="Y49" r:id="rId213"/>
+    <hyperlink ref="AI49" r:id="rId214"/>
+    <hyperlink ref="AN49" r:id="rId215"/>
+    <hyperlink ref="G50" r:id="rId216"/>
+    <hyperlink ref="T50" r:id="rId217"/>
+    <hyperlink ref="Y50" r:id="rId218"/>
+    <hyperlink ref="AI50" r:id="rId219"/>
+    <hyperlink ref="AN50" r:id="rId220"/>
+    <hyperlink ref="G51" r:id="rId221"/>
+    <hyperlink ref="T51" r:id="rId222"/>
+    <hyperlink ref="AD51" r:id="rId223"/>
+    <hyperlink ref="AI51" r:id="rId224"/>
+    <hyperlink ref="K53" r:id="rId225"/>
+    <hyperlink ref="P53" r:id="rId226"/>
+    <hyperlink ref="U53" r:id="rId227"/>
+    <hyperlink ref="Z53" r:id="rId228"/>
+    <hyperlink ref="AE53" r:id="rId229"/>
+    <hyperlink ref="AJ53" r:id="rId230"/>
+    <hyperlink ref="AO53" r:id="rId231"/>
+    <hyperlink ref="AT53" r:id="rId232"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId232"/>
+  <legacyDrawing r:id="rId233"/>
 </worksheet>
 </file>
</xml_diff>